<commit_message>
Update data to June 2025 and retrain models
</commit_message>
<xml_diff>
--- a/NaturalGasPrice_Input.xlsx
+++ b/NaturalGasPrice_Input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://transgraph-my.sharepoint.com/personal/sasikumar_m_transgraph_com/Documents/Desktop/Sasi's WorkSpace/FY 2025-2026/June2025/HenryHub Demand and Prices/Price/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ML Projects\ML_2025\Natural_Gas_Price_June2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="11_F25DC773A252ABDACC1048FCB95D52365ADE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48235ED7-3F73-4626-B89C-BF933902593B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C33E92F-8F02-4EC4-8423-EA79CBD1A4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -182,7 +182,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{0547865B-E5AC-445C-93BA-8EE69815A116}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -192,10 +194,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -464,26 +462,26 @@
   <dimension ref="A1:K256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B173" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomRight" activeCell="M174" sqref="M174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" customWidth="1"/>
+    <col min="8" max="8" width="15.54296875" customWidth="1"/>
+    <col min="9" max="9" width="10.26953125" customWidth="1"/>
+    <col min="10" max="10" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -515,7 +513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>40179</v>
       </c>
@@ -547,7 +545,7 @@
         <v>5.5988947368421051</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>40210</v>
       </c>
@@ -579,7 +577,7 @@
         <v>5.2139999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>40238</v>
       </c>
@@ -611,7 +609,7 @@
         <v>4.2999999999999989</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>40269</v>
       </c>
@@ -643,7 +641,7 @@
         <v>4.0836190476190479</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>40299</v>
       </c>
@@ -675,7 +673,7 @@
         <v>4.1540499999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>40330</v>
       </c>
@@ -707,7 +705,7 @@
         <v>4.7837727272727273</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>40360</v>
       </c>
@@ -739,7 +737,7 @@
         <v>4.5899523809523801</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>40391</v>
       </c>
@@ -771,7 +769,7 @@
         <v>4.2178181818181821</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>40422</v>
       </c>
@@ -803,7 +801,7 @@
         <v>3.8967619047619046</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>40452</v>
       </c>
@@ -835,7 +833,7 @@
         <v>3.5996190476190475</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>40483</v>
       </c>
@@ -867,7 +865,7 @@
         <v>4.0407619047619043</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>40513</v>
       </c>
@@ -899,7 +897,7 @@
         <v>4.2818181818181822</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>40544</v>
       </c>
@@ -931,7 +929,7 @@
         <v>4.4982999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>40575</v>
       </c>
@@ -963,7 +961,7 @@
         <v>4.0355263157894736</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>40603</v>
       </c>
@@ -995,7 +993,7 @@
         <v>4.0692173913043481</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>40634</v>
       </c>
@@ -1027,7 +1025,7 @@
         <v>4.2716499999999993</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>40664</v>
       </c>
@@ -1059,7 +1057,7 @@
         <v>4.3361428571428569</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>40695</v>
       </c>
@@ -1091,7 +1089,7 @@
         <v>4.5160454545454547</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>40725</v>
       </c>
@@ -1123,7 +1121,7 @@
         <v>4.3532500000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>40756</v>
       </c>
@@ -1155,7 +1153,7 @@
         <v>3.9835652173913045</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>40787</v>
       </c>
@@ -1187,7 +1185,7 @@
         <v>3.8490476190476182</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>40817</v>
       </c>
@@ -1219,7 +1217,7 @@
         <v>3.6239523809523808</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>40848</v>
       </c>
@@ -1251,7 +1249,7 @@
         <v>3.5577142857142858</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>40878</v>
       </c>
@@ -1283,7 +1281,7 @@
         <v>3.2462857142857149</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>40909</v>
       </c>
@@ -1315,7 +1313,7 @@
         <v>2.7077999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>40940</v>
       </c>
@@ -1347,7 +1345,7 @@
         <v>2.5259499999999995</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>40969</v>
       </c>
@@ -1379,7 +1377,7 @@
         <v>2.2955909090909086</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>41000</v>
       </c>
@@ -1411,7 +1409,7 @@
         <v>2.0482000000000005</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>41030</v>
       </c>
@@ -1443,7 +1441,7 @@
         <v>2.4934090909090907</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>41061</v>
       </c>
@@ -1475,7 +1473,7 @@
         <v>2.4982380952380958</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>41091</v>
       </c>
@@ -1507,7 +1505,7 @@
         <v>2.9631904761904759</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>41122</v>
       </c>
@@ -1539,7 +1537,7 @@
         <v>2.8074347826086954</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>41153</v>
       </c>
@@ -1571,7 +1569,7 @@
         <v>2.917736842105263</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>41183</v>
       </c>
@@ -1603,7 +1601,7 @@
         <v>3.4995652173913046</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>41214</v>
       </c>
@@ -1635,7 +1633,7 @@
         <v>3.6873333333333331</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>41244</v>
       </c>
@@ -1667,7 +1665,7 @@
         <v>3.4441500000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>41275</v>
       </c>
@@ -1699,7 +1697,7 @@
         <v>3.3499523809523812</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>41306</v>
       </c>
@@ -1731,7 +1729,7 @@
         <v>3.3142105263157888</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>41334</v>
       </c>
@@ -1763,7 +1761,7 @@
         <v>3.7729500000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>41365</v>
       </c>
@@ -1795,7 +1793,7 @@
         <v>4.1611363636363627</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>41395</v>
       </c>
@@ -1827,7 +1825,7 @@
         <v>4.0679545454545449</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>41426</v>
       </c>
@@ -1859,7 +1857,7 @@
         <v>3.8061999999999996</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>41456</v>
       </c>
@@ -1891,7 +1889,7 @@
         <v>3.6412727272727277</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>41487</v>
       </c>
@@ -1923,7 +1921,7 @@
         <v>3.4126363636363637</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>41518</v>
       </c>
@@ -1955,7 +1953,7 @@
         <v>3.6180999999999996</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>41548</v>
       </c>
@@ -1987,7 +1985,7 @@
         <v>3.6543478260869571</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>41579</v>
       </c>
@@ -2019,7 +2017,7 @@
         <v>3.6397499999999994</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>41609</v>
       </c>
@@ -2051,7 +2049,7 @@
         <v>4.2765238095238098</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>41640</v>
       </c>
@@ -2083,7 +2081,7 @@
         <v>4.5525238095238096</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>41671</v>
       </c>
@@ -2115,7 +2113,7 @@
         <v>5.162789473684211</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>41699</v>
       </c>
@@ -2147,7 +2145,7 @@
         <v>4.4858571428571432</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>41730</v>
       </c>
@@ -2179,7 +2177,7 @@
         <v>4.608428571428572</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>41760</v>
       </c>
@@ -2211,7 +2209,7 @@
         <v>4.535619047619047</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>41791</v>
       </c>
@@ -2243,7 +2241,7 @@
         <v>4.593809523809524</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>41821</v>
       </c>
@@ -2275,7 +2273,7 @@
         <v>4.0247272727272723</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>41852</v>
       </c>
@@ -2307,7 +2305,7 @@
         <v>3.8993809523809517</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>41883</v>
       </c>
@@ -2339,7 +2337,7 @@
         <v>3.9207619047619042</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>41913</v>
       </c>
@@ -2371,7 +2369,7 @@
         <v>3.8010869565217384</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>41944</v>
       </c>
@@ -2403,7 +2401,7 @@
         <v>4.2345263157894735</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>41974</v>
       </c>
@@ -2435,7 +2433,7 @@
         <v>3.5085909090909082</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>42005</v>
       </c>
@@ -2467,7 +2465,7 @@
         <v>2.9274285714285719</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>42036</v>
       </c>
@@ -2499,7 +2497,7 @@
         <v>2.7549473684210533</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>42064</v>
       </c>
@@ -2531,7 +2529,7 @@
         <v>2.7469090909090905</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>42095</v>
       </c>
@@ -2563,7 +2561,7 @@
         <v>2.5968636363636368</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>42125</v>
       </c>
@@ -2595,7 +2593,7 @@
         <v>2.85595</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>42156</v>
       </c>
@@ -2627,7 +2625,7 @@
         <v>2.7692272727272726</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>42186</v>
       </c>
@@ -2659,7 +2657,7 @@
         <v>2.8080909090909092</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>42217</v>
       </c>
@@ -2691,7 +2689,7 @@
         <v>2.7534761904761904</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>42248</v>
       </c>
@@ -2723,7 +2721,7 @@
         <v>2.6389047619047621</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>42278</v>
       </c>
@@ -2755,7 +2753,7 @@
         <v>2.385045454545454</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>42309</v>
       </c>
@@ -2787,7 +2785,7 @@
         <v>2.2798500000000006</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>42339</v>
       </c>
@@ -2819,7 +2817,7 @@
         <v>2.0434999999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>42370</v>
       </c>
@@ -2851,7 +2849,7 @@
         <v>2.2333684210526314</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>42401</v>
       </c>
@@ -2883,7 +2881,7 @@
         <v>1.9294499999999997</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>42430</v>
       </c>
@@ -2915,7 +2913,7 @@
         <v>1.8121363636363634</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>42461</v>
       </c>
@@ -2947,7 +2945,7 @@
         <v>2.0143809523809524</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>42491</v>
       </c>
@@ -2979,7 +2977,7 @@
         <v>2.0834285714285712</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>42522</v>
       </c>
@@ -3011,7 +3009,7 @@
         <v>2.6238181818181818</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>42552</v>
       </c>
@@ -3043,7 +3041,7 @@
         <v>2.7614000000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>42583</v>
       </c>
@@ -3075,7 +3073,7 @@
         <v>2.7223478260869567</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>42614</v>
       </c>
@@ -3107,7 +3105,7 @@
         <v>2.9029047619047619</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>42644</v>
       </c>
@@ -3139,7 +3137,7 @@
         <v>3.0742857142857152</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>42675</v>
       </c>
@@ -3171,7 +3169,7 @@
         <v>2.8728571428571428</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>42705</v>
       </c>
@@ -3203,7 +3201,7 @@
         <v>3.5837142857142861</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>42736</v>
       </c>
@@ -3235,7 +3233,7 @@
         <v>3.2911999999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>42767</v>
       </c>
@@ -3267,7 +3265,7 @@
         <v>2.9067368421052633</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>42795</v>
       </c>
@@ -3299,7 +3297,7 @@
         <v>2.9924347826086954</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>42826</v>
       </c>
@@ -3331,7 +3329,7 @@
         <v>3.1894736842105269</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>42856</v>
       </c>
@@ -3363,7 +3361,7 @@
         <v>3.2356363636363636</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>42887</v>
       </c>
@@ -3395,7 +3393,7 @@
         <v>2.9935909090909094</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>42917</v>
       </c>
@@ -3427,7 +3425,7 @@
         <v>2.9551500000000002</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>42948</v>
       </c>
@@ -3459,7 +3457,7 @@
         <v>2.9051739130434782</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>42979</v>
       </c>
@@ -3491,7 +3489,7 @@
         <v>3.0058999999999996</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>43009</v>
       </c>
@@ -3523,7 +3521,7 @@
         <v>2.912590909090909</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>43040</v>
       </c>
@@ -3555,7 +3553,7 @@
         <v>3.0588571428571432</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>43070</v>
       </c>
@@ -3587,7 +3585,7 @@
         <v>2.7760500000000001</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>43101</v>
       </c>
@@ -3619,7 +3617,7 @@
         <v>3.160571428571429</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>43132</v>
       </c>
@@ -3651,7 +3649,7 @@
         <v>2.6623684210526317</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>43160</v>
       </c>
@@ -3683,7 +3681,7 @@
         <v>2.6993809523809524</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
         <v>43191</v>
       </c>
@@ -3715,7 +3713,7 @@
         <v>2.7242380952380949</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>43221</v>
       </c>
@@ -3747,7 +3745,7 @@
         <v>2.8293181818181821</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="5">
         <v>43252</v>
       </c>
@@ -3779,7 +3777,7 @@
         <v>2.9425238095238098</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" s="5">
         <v>43282</v>
       </c>
@@ -3811,7 +3809,7 @@
         <v>2.7893333333333339</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>43313</v>
       </c>
@@ -3843,7 +3841,7 @@
         <v>2.9080869565217391</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" s="5">
         <v>43344</v>
       </c>
@@ -3875,7 +3873,7 @@
         <v>2.8959999999999995</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
         <v>43374</v>
       </c>
@@ -3907,7 +3905,7 @@
         <v>3.2079565217391299</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" s="5">
         <v>43405</v>
       </c>
@@ -3939,7 +3937,7 @@
         <v>4.0933809523809526</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="5">
         <v>43435</v>
       </c>
@@ -3971,7 +3969,7 @@
         <v>3.9252499999999997</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" s="5">
         <v>43466</v>
       </c>
@@ -4003,7 +4001,7 @@
         <v>3.1003333333333334</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" s="5">
         <v>43497</v>
       </c>
@@ -4035,7 +4033,7 @@
         <v>2.682578947368421</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="5">
         <v>43525</v>
       </c>
@@ -4067,7 +4065,7 @@
         <v>2.8046666666666669</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" s="5">
         <v>43556</v>
       </c>
@@ -4099,7 +4097,7 @@
         <v>2.6030952380952392</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="5">
         <v>43586</v>
       </c>
@@ -4131,7 +4129,7 @@
         <v>2.5924090909090904</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" s="5">
         <v>43617</v>
       </c>
@@ -4163,7 +4161,7 @@
         <v>2.3303499999999997</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" s="5">
         <v>43647</v>
       </c>
@@ -4195,7 +4193,7 @@
         <v>2.3030909090909084</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" s="5">
         <v>43678</v>
       </c>
@@ -4227,7 +4225,7 @@
         <v>2.1742727272727267</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" s="5">
         <v>43709</v>
       </c>
@@ -4259,7 +4257,7 @@
         <v>2.5195499999999997</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" s="5">
         <v>43739</v>
       </c>
@@ -4291,7 +4289,7 @@
         <v>2.3392608695652171</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="5">
         <v>43770</v>
       </c>
@@ -4323,7 +4321,7 @@
         <v>2.6314499999999996</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" s="5">
         <v>43800</v>
       </c>
@@ -4355,7 +4353,7 @@
         <v>2.288238095238095</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" s="5">
         <v>43831</v>
       </c>
@@ -4387,7 +4385,7 @@
         <v>2.0356956521739131</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="5">
         <v>43862</v>
       </c>
@@ -4419,7 +4417,7 @@
         <v>1.8431000000000002</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" s="5">
         <v>43891</v>
       </c>
@@ -4451,7 +4449,7 @@
         <v>1.7311818181818177</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" s="5">
         <v>43922</v>
       </c>
@@ -4483,7 +4481,7 @@
         <v>1.7581363636363634</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" s="5">
         <v>43952</v>
       </c>
@@ -4515,7 +4513,7 @@
         <v>1.8054285714285716</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" s="5">
         <v>43983</v>
       </c>
@@ -4547,7 +4545,7 @@
         <v>1.7008636363636365</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" s="5">
         <v>44013</v>
       </c>
@@ -4579,7 +4577,7 @@
         <v>1.7636086956521737</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" s="5">
         <v>44044</v>
       </c>
@@ -4611,7 +4609,7 @@
         <v>2.3434761904761907</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" s="5">
         <v>44075</v>
       </c>
@@ -4643,7 +4641,7 @@
         <v>2.294227272727273</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" s="5">
         <v>44105</v>
       </c>
@@ -4675,7 +4673,7 @@
         <v>2.8362272727272724</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" s="5">
         <v>44136</v>
       </c>
@@ -4707,7 +4705,7 @@
         <v>2.8730952380952379</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" s="5">
         <v>44166</v>
       </c>
@@ -4739,7 +4737,7 @@
         <v>2.581391304347826</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" s="5">
         <v>44197</v>
       </c>
@@ -4771,7 +4769,7 @@
         <v>2.6477142857142857</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" s="5">
         <v>44228</v>
       </c>
@@ -4803,7 +4801,7 @@
         <v>2.9167500000000004</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" s="5">
         <v>44256</v>
       </c>
@@ -4835,7 +4833,7 @@
         <v>2.6220434782608693</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" s="5">
         <v>44287</v>
       </c>
@@ -4867,7 +4865,7 @@
         <v>2.6829999999999994</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" s="5">
         <v>44317</v>
       </c>
@@ -4899,7 +4897,7 @@
         <v>2.9607619047619043</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" s="5">
         <v>44348</v>
       </c>
@@ -4931,7 +4929,7 @@
         <v>3.2724090909090915</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" s="5">
         <v>44378</v>
       </c>
@@ -4963,7 +4961,7 @@
         <v>3.8098181818181813</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" s="5">
         <v>44409</v>
       </c>
@@ -4995,7 +4993,7 @@
         <v>4.0314545454545447</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" s="5">
         <v>44440</v>
       </c>
@@ -5027,7 +5025,7 @@
         <v>5.0965454545454554</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" s="5">
         <v>44470</v>
       </c>
@@ -5059,7 +5057,7 @@
         <v>5.5706190476190471</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" s="5">
         <v>44501</v>
       </c>
@@ -5091,7 +5089,7 @@
         <v>5.1178636363636372</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" s="5">
         <v>44531</v>
       </c>
@@ -5123,7 +5121,7 @@
         <v>3.8580434782608695</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" s="5">
         <v>44562</v>
       </c>
@@ -5155,7 +5153,7 @@
         <v>4.2554499999999997</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" s="5">
         <v>44593</v>
       </c>
@@ -5187,7 +5185,7 @@
         <v>4.4630000000000001</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" s="5">
         <v>44621</v>
       </c>
@@ -5219,7 +5217,7 @@
         <v>4.979304347826087</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" s="5">
         <v>44652</v>
       </c>
@@ -5251,7 +5249,7 @@
         <v>6.7045999999999992</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" s="5">
         <v>44682</v>
       </c>
@@ -5283,7 +5281,7 @@
         <v>8.1634761904761906</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" s="5">
         <v>44713</v>
       </c>
@@ -5315,7 +5313,7 @@
         <v>7.5979047619047613</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" s="5">
         <v>44743</v>
       </c>
@@ -5347,7 +5345,7 @@
         <v>7.1869499999999986</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" s="5">
         <v>44774</v>
       </c>
@@ -5379,7 +5377,7 @@
         <v>8.779478260869567</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" s="5">
         <v>44805</v>
       </c>
@@ -5411,7 +5409,7 @@
         <v>7.7575238095238088</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" s="5">
         <v>44835</v>
       </c>
@@ -5443,7 +5441,7 @@
         <v>6.0849047619047623</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" s="5">
         <v>44866</v>
       </c>
@@ -5475,7 +5473,7 @@
         <v>6.4297619047619055</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157" s="5">
         <v>44896</v>
       </c>
@@ -5507,7 +5505,7 @@
         <v>5.7680476190476169</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158" s="5">
         <v>44927</v>
       </c>
@@ -5539,7 +5537,7 @@
         <v>3.4228000000000001</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159" s="5">
         <v>44958</v>
       </c>
@@ -5571,7 +5569,7 @@
         <v>2.4374736842105262</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160" s="5">
         <v>44986</v>
       </c>
@@ -5603,7 +5601,7 @@
         <v>2.4077826086956522</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161" s="5">
         <v>45017</v>
       </c>
@@ -5635,7 +5633,7 @@
         <v>2.1972631578947373</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A162" s="5">
         <v>45047</v>
       </c>
@@ -5667,7 +5665,7 @@
         <v>2.2993181818181814</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163" s="5">
         <v>45078</v>
       </c>
@@ -5699,7 +5697,7 @@
         <v>2.4746190476190475</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A164" s="5">
         <v>45108</v>
       </c>
@@ -5731,7 +5729,7 @@
         <v>2.6365500000000002</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A165" s="5">
         <v>45139</v>
       </c>
@@ -5763,7 +5761,7 @@
         <v>2.6451304347826086</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A166" s="5">
         <v>45170</v>
       </c>
@@ -5795,7 +5793,7 @@
         <v>2.6956500000000001</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A167" s="5">
         <v>45200</v>
       </c>
@@ -5827,7 +5825,7 @@
         <v>3.1491818181818179</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A168" s="5">
         <v>45231</v>
       </c>
@@ -5859,7 +5857,7 @@
         <v>3.0555238095238093</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A169" s="5">
         <v>45261</v>
       </c>
@@ -5891,7 +5889,7 @@
         <v>2.5388500000000005</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A170" s="5">
         <v>45292</v>
       </c>
@@ -5923,7 +5921,7 @@
         <v>2.7149999999999999</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A171" s="5">
         <v>45323</v>
       </c>
@@ -5955,7 +5953,7 @@
         <v>1.7954999999999999</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A172" s="5">
         <v>45352</v>
       </c>
@@ -5987,7 +5985,7 @@
         <v>1.7472999999999999</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A173" s="5">
         <v>45383</v>
       </c>
@@ -6019,7 +6017,7 @@
         <v>1.7912272727272727</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A174" s="5">
         <v>45413</v>
       </c>
@@ -6051,7 +6049,7 @@
         <v>2.4180000000000001</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A175" s="5">
         <v>45444</v>
       </c>
@@ -6083,7 +6081,7 @@
         <v>2.8095789473684207</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A176" s="5">
         <v>45474</v>
       </c>
@@ -6115,7 +6113,7 @@
         <v>2.2086818181818177</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A177" s="5">
         <v>45505</v>
       </c>
@@ -6147,7 +6145,7 @@
         <v>2.0867826086956525</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A178" s="5">
         <v>45536</v>
       </c>
@@ -6179,7 +6177,7 @@
         <v>2.4092500000000006</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A179" s="5">
         <v>45566</v>
       </c>
@@ -6211,7 +6209,7 @@
         <v>2.5769565217391306</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A180" s="5">
         <v>45597</v>
       </c>
@@ -6243,7 +6241,7 @@
         <v>2.9819999999999998</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A181" s="5">
         <v>45627</v>
       </c>
@@ -6275,7 +6273,7 @@
         <v>3.4066190476190479</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A182" s="5">
         <v>45658</v>
       </c>
@@ -6307,7 +6305,7 @@
         <v>3.7213809523809522</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A183" s="5">
         <v>45689</v>
       </c>
@@ -6339,7 +6337,7 @@
         <v>3.7409473684210526</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A184" s="5">
         <v>45717</v>
       </c>
@@ -6361,233 +6359,320 @@
       <c r="G184" s="4">
         <v>7.905710758400005</v>
       </c>
-      <c r="H184" s="6">
+      <c r="H184" s="4">
         <v>5.0205686399999998E-2</v>
       </c>
-      <c r="I184" s="6">
+      <c r="I184" s="4">
         <v>21.331300291200002</v>
       </c>
       <c r="J184" s="4">
         <v>4.1374761904761908</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J185" s="7"/>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A185" s="5">
+        <v>45748</v>
+      </c>
+      <c r="B185" s="4">
+        <v>111.3</v>
+      </c>
+      <c r="C185" s="4">
+        <v>16.2</v>
+      </c>
+      <c r="D185" s="4">
+        <v>7.3</v>
+      </c>
+      <c r="E185" s="4">
+        <v>21</v>
+      </c>
+      <c r="F185" s="4">
+        <v>23.9</v>
+      </c>
+      <c r="G185" s="4">
+        <v>7.6</v>
+      </c>
+      <c r="H185" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I185" s="4">
+        <v>20.8</v>
+      </c>
+      <c r="J185" s="4">
+        <v>3.4</v>
+      </c>
       <c r="K185" s="7"/>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J186" s="7"/>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A186" s="5">
+        <v>45778</v>
+      </c>
+      <c r="B186" s="4">
+        <v>114.4</v>
+      </c>
+      <c r="C186" s="4">
+        <v>10.1</v>
+      </c>
+      <c r="D186" s="4">
+        <v>5.4</v>
+      </c>
+      <c r="E186" s="4">
+        <v>20.2</v>
+      </c>
+      <c r="F186" s="4">
+        <v>25.3</v>
+      </c>
+      <c r="G186" s="4">
+        <v>7.6</v>
+      </c>
+      <c r="H186" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I186" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="J186" s="4">
+        <v>3.5</v>
+      </c>
       <c r="K186" s="7"/>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J187" s="7"/>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A187" s="5">
+        <v>45809</v>
+      </c>
+      <c r="B187" s="4">
+        <v>113.5</v>
+      </c>
+      <c r="C187" s="4">
+        <v>5.6</v>
+      </c>
+      <c r="D187" s="4">
+        <v>4.3</v>
+      </c>
+      <c r="E187" s="4">
+        <v>19.8</v>
+      </c>
+      <c r="F187" s="4">
+        <v>33.1</v>
+      </c>
+      <c r="G187" s="4">
+        <v>7.4</v>
+      </c>
+      <c r="H187" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I187" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="J187" s="4">
+        <v>3.7</v>
+      </c>
       <c r="K187" s="7"/>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K188" s="7"/>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K189" s="7"/>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K190" s="7"/>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K191" s="7"/>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K192" s="7"/>
     </row>
-    <row r="193" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="193" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K193" s="7"/>
     </row>
-    <row r="194" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="194" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K194" s="7"/>
     </row>
-    <row r="195" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="195" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K195" s="7"/>
     </row>
-    <row r="196" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="196" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K196" s="7"/>
     </row>
-    <row r="197" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="197" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K197" s="7"/>
     </row>
-    <row r="198" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="198" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K198" s="7"/>
     </row>
-    <row r="199" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="199" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K199" s="7"/>
     </row>
-    <row r="200" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="200" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K200" s="7"/>
     </row>
-    <row r="201" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="201" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K201" s="7"/>
     </row>
-    <row r="202" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="202" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K202" s="7"/>
     </row>
-    <row r="203" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="203" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K203" s="7"/>
     </row>
-    <row r="204" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="204" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K204" s="7"/>
     </row>
-    <row r="205" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="205" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K205" s="7"/>
     </row>
-    <row r="206" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="206" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K206" s="7"/>
     </row>
-    <row r="207" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="207" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K207" s="7"/>
     </row>
-    <row r="208" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="208" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K208" s="7"/>
     </row>
-    <row r="209" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="209" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K209" s="7"/>
     </row>
-    <row r="210" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="210" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K210" s="7"/>
     </row>
-    <row r="211" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="211" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K211" s="7"/>
     </row>
-    <row r="212" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="212" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K212" s="7"/>
     </row>
-    <row r="213" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="213" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K213" s="7"/>
     </row>
-    <row r="214" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="214" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K214" s="7"/>
     </row>
-    <row r="215" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="215" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K215" s="7"/>
     </row>
-    <row r="216" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="216" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K216" s="7"/>
     </row>
-    <row r="217" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="217" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K217" s="7"/>
     </row>
-    <row r="218" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="218" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K218" s="7"/>
     </row>
-    <row r="219" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="219" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K219" s="7"/>
     </row>
-    <row r="220" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="220" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K220" s="7"/>
     </row>
-    <row r="221" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="221" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K221" s="7"/>
     </row>
-    <row r="222" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="222" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K222" s="7"/>
     </row>
-    <row r="223" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="223" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K223" s="7"/>
     </row>
-    <row r="224" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="224" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K224" s="7"/>
     </row>
-    <row r="225" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="225" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K225" s="7"/>
     </row>
-    <row r="226" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="226" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K226" s="7"/>
     </row>
-    <row r="227" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="227" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K227" s="7"/>
     </row>
-    <row r="228" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="228" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K228" s="7"/>
     </row>
-    <row r="229" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="229" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K229" s="7"/>
     </row>
-    <row r="230" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="230" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K230" s="7"/>
     </row>
-    <row r="231" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="231" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K231" s="7"/>
     </row>
-    <row r="232" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="232" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K232" s="7"/>
     </row>
-    <row r="233" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="233" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K233" s="7"/>
     </row>
-    <row r="234" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="234" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K234" s="7"/>
     </row>
-    <row r="235" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="235" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K235" s="7"/>
     </row>
-    <row r="236" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="236" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K236" s="7"/>
     </row>
-    <row r="237" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="237" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K237" s="7"/>
     </row>
-    <row r="238" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="238" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K238" s="7"/>
     </row>
-    <row r="239" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="239" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K239" s="7"/>
     </row>
-    <row r="240" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="240" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K240" s="7"/>
     </row>
-    <row r="241" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="241" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K241" s="7"/>
     </row>
-    <row r="242" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="242" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K242" s="7"/>
     </row>
-    <row r="243" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="243" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K243" s="7"/>
     </row>
-    <row r="244" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="244" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K244" s="7"/>
     </row>
-    <row r="245" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="245" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K245" s="7"/>
     </row>
-    <row r="246" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="246" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K246" s="7"/>
     </row>
-    <row r="247" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="247" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K247" s="7"/>
     </row>
-    <row r="248" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="248" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K248" s="7"/>
     </row>
-    <row r="249" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="249" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K249" s="7"/>
     </row>
-    <row r="250" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="250" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K250" s="7"/>
     </row>
-    <row r="251" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="251" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K251" s="7"/>
     </row>
-    <row r="252" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="252" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K252" s="7"/>
     </row>
-    <row r="253" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="253" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K253" s="7"/>
     </row>
-    <row r="254" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="254" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K254" s="7"/>
     </row>
-    <row r="255" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="255" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K255" s="7"/>
     </row>
-    <row r="256" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="256" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K256" s="7"/>
     </row>
   </sheetData>

</xml_diff>